<commit_message>
Fixed experimental11 test so it passes with new framework.
</commit_message>
<xml_diff>
--- a/t/regression/xlsx_files/experimental11.xlsx
+++ b/t/regression/xlsx_files/experimental11.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -169,14 +169,14 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-2700000" vert="horz"/>
+              <a:bodyPr rot="2700000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr baseline="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" baseline="0"/>
                   <a:t>XXX</a:t>
                 </a:r>
               </a:p>

</xml_diff>